<commit_message>
Mise à jour du rapport
</commit_message>
<xml_diff>
--- a/Documentation/Versions originaux/Journal de travail.xlsx
+++ b/Documentation/Versions originaux/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\TPI\Documentation\Versions originaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354BE3DC-AF40-4E65-9839-41350478362B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6E9A9E-E341-4ED8-B4E5-228783A2C1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Jour</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>Se documenter et créer le panier et l'ajout des biscuits</t>
+  </si>
+  <si>
+    <t>Créer la page de profil et afficher les informations personnelles</t>
+  </si>
+  <si>
+    <t>Créer un formulaire permettant de modifier les informations du compte et afficher les nouvelles données</t>
+  </si>
+  <si>
+    <t>Finir de mettre en place le panier et l'ajout des produits depuis la page des détails</t>
+  </si>
+  <si>
+    <t>Mettre à jour le rapport de projet</t>
   </si>
 </sst>
 </file>
@@ -538,7 +550,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,37 +978,77 @@
       </c>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>45057</v>
+      </c>
+      <c r="B24" s="7">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>45057</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>45057</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
+      <c r="A27" s="6">
+        <v>45058</v>
+      </c>
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>

</xml_diff>

<commit_message>
Création de la page d'administration
</commit_message>
<xml_diff>
--- a/Documentation/Versions originaux/Journal de travail.xlsx
+++ b/Documentation/Versions originaux/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\TPI\Documentation\Versions originaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6E9A9E-E341-4ED8-B4E5-228783A2C1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFE1F6F-C22B-46F3-8A56-7915DD28559A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>Jour</t>
   </si>
@@ -139,6 +139,33 @@
   </si>
   <si>
     <t>Mettre à jour le rapport de projet</t>
+  </si>
+  <si>
+    <t>Avancer sur la page des commandes du client</t>
+  </si>
+  <si>
+    <t>Héberger une partie du site sur SwissCenter</t>
+  </si>
+  <si>
+    <t>Srpint Review</t>
+  </si>
+  <si>
+    <t>Ajouter des stratgies de test dans le rappot</t>
+  </si>
+  <si>
+    <t>Améliorer l'aspect graphique du site</t>
+  </si>
+  <si>
+    <t>Envoyer les données du panier vers la page des commandes</t>
+  </si>
+  <si>
+    <t>Créer la page administrateur et afficher les biscuits</t>
+  </si>
+  <si>
+    <t>Coder l'ajout de produit et la modification</t>
+  </si>
+  <si>
+    <t>Finaliser la modification des biscuits</t>
   </si>
 </sst>
 </file>
@@ -549,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,76 +1078,166 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17"/>
+      <c r="A28" s="6">
+        <v>45058</v>
+      </c>
+      <c r="B28" s="7">
+        <v>2</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
+      <c r="A29" s="6">
+        <v>45058</v>
+      </c>
+      <c r="B29" s="7">
+        <v>2</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
+      <c r="A30" s="6">
+        <v>45058</v>
+      </c>
+      <c r="B30" s="7">
+        <v>2</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17"/>
+      <c r="A31" s="6">
+        <v>45058</v>
+      </c>
+      <c r="B31" s="7">
+        <v>2</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="17"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
+      <c r="A32" s="6">
+        <v>45061</v>
+      </c>
+      <c r="B32" s="7">
+        <v>3</v>
+      </c>
+      <c r="C32" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>45061</v>
+      </c>
+      <c r="B33" s="7">
+        <v>3</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="17"/>
+      <c r="A34" s="6">
+        <v>45061</v>
+      </c>
+      <c r="B34" s="7">
+        <v>3</v>
+      </c>
+      <c r="C34" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="17"/>
+      <c r="A35" s="6">
+        <v>45061</v>
+      </c>
+      <c r="B35" s="7">
+        <v>3</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="17"/>
+      <c r="A36" s="6">
+        <v>45062</v>
+      </c>
+      <c r="B36" s="7">
+        <v>3</v>
+      </c>
+      <c r="C36" s="8">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>

</xml_diff>

<commit_message>
Affichage de la liste des commandes
</commit_message>
<xml_diff>
--- a/Documentation/Versions originaux/Journal de travail.xlsx
+++ b/Documentation/Versions originaux/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\TPI\Documentation\Versions originaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFE1F6F-C22B-46F3-8A56-7915DD28559A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB34951-08B7-4620-88CA-7A1AD32DFD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>Jour</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>Finaliser la modification des biscuits</t>
+  </si>
+  <si>
+    <t>Avancer sur la documentation</t>
+  </si>
+  <si>
+    <t>Modifier le MCD et le MLD et la liste des commandes</t>
+  </si>
+  <si>
+    <t>Finaliser la liste des commandes des clients</t>
+  </si>
+  <si>
+    <t>Entretien avec le 2ème expert</t>
+  </si>
+  <si>
+    <t>Améliorer le frontend de la liste des commandes et du gabarit</t>
   </si>
 </sst>
 </file>
@@ -236,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -274,26 +289,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,44 +1235,94 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="17"/>
+      <c r="A37" s="6">
+        <v>45062</v>
+      </c>
+      <c r="B37" s="7">
+        <v>3</v>
+      </c>
+      <c r="C37" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="17"/>
+      <c r="A38" s="6">
+        <v>45062</v>
+      </c>
+      <c r="B38" s="7">
+        <v>3</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17"/>
+      <c r="A39" s="6">
+        <v>45062</v>
+      </c>
+      <c r="B39" s="7">
+        <v>3</v>
+      </c>
+      <c r="C39" s="8">
+        <v>2.75</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="17"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17"/>
+      <c r="A40" s="6">
+        <v>45062</v>
+      </c>
+      <c r="B40" s="7">
+        <v>3</v>
+      </c>
+      <c r="C40" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>45068</v>
+      </c>
+      <c r="B41" s="7">
+        <v>4</v>
+      </c>
+      <c r="C41" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" s="11"/>

</xml_diff>

<commit_message>
Menu filtre de la boutique
</commit_message>
<xml_diff>
--- a/Documentation/Versions originaux/Journal de travail.xlsx
+++ b/Documentation/Versions originaux/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\TPI\Documentation\Versions originaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9149A5AF-40BF-487A-BD32-136B40EA44C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B03D86E-7FD0-457C-B36E-1AF0DCA4209A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>Jour</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Mettre en place l'activation et la désactivation d'un produit</t>
+  </si>
+  <si>
+    <t>Créer un menu de filtre sur la page boutique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valider les commandes du panier et envoyer les données dans la base de donées </t>
   </si>
 </sst>
 </file>
@@ -595,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,6 +1428,78 @@
       </c>
       <c r="F45" s="5"/>
     </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>45068</v>
+      </c>
+      <c r="B46" s="7">
+        <v>4</v>
+      </c>
+      <c r="C46" s="8">
+        <v>1</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>45069</v>
+      </c>
+      <c r="B47" s="7">
+        <v>4</v>
+      </c>
+      <c r="C47" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>45069</v>
+      </c>
+      <c r="B48" s="7">
+        <v>4</v>
+      </c>
+      <c r="C48" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>45069</v>
+      </c>
+      <c r="B49" s="7">
+        <v>4</v>
+      </c>
+      <c r="C49" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Page d'accueil à jour
</commit_message>
<xml_diff>
--- a/Documentation/Versions originaux/Journal de travail.xlsx
+++ b/Documentation/Versions originaux/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\TPI\Documentation\Versions originaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B03D86E-7FD0-457C-B36E-1AF0DCA4209A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E438C68-7BB7-4ACA-8465-779C7CF2297D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="1785" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
   <si>
     <t>Jour</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t xml:space="preserve">Valider les commandes du panier et envoyer les données dans la base de donées </t>
+  </si>
+  <si>
+    <t>Corriger des erreurs d'affichage des informations de l'utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vérifier le fonctionnement générale du site </t>
+  </si>
+  <si>
+    <t>Ajouter du contenu à la page d'accueil et modifier la page boutique</t>
+  </si>
+  <si>
+    <t>Mettre la nouvelle version sur SwissCenter</t>
   </si>
 </sst>
 </file>
@@ -601,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,6 +1512,114 @@
       </c>
       <c r="F49" s="5"/>
     </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>45071</v>
+      </c>
+      <c r="B50" s="7">
+        <v>4</v>
+      </c>
+      <c r="C50" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>45071</v>
+      </c>
+      <c r="B51" s="7">
+        <v>4</v>
+      </c>
+      <c r="C51" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>45071</v>
+      </c>
+      <c r="B52" s="7">
+        <v>4</v>
+      </c>
+      <c r="C52" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>45072</v>
+      </c>
+      <c r="B53" s="7">
+        <v>4</v>
+      </c>
+      <c r="C53" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>45072</v>
+      </c>
+      <c r="B54" s="7">
+        <v>4</v>
+      </c>
+      <c r="C54" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>45072</v>
+      </c>
+      <c r="B55" s="7">
+        <v>4</v>
+      </c>
+      <c r="C55" s="8">
+        <v>1</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F55" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Fin de Sprint 3
</commit_message>
<xml_diff>
--- a/Documentation/Versions originaux/Journal de travail.xlsx
+++ b/Documentation/Versions originaux/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\TPI\Documentation\Versions originaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E438C68-7BB7-4ACA-8465-779C7CF2297D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68AF53B-6D06-4DC1-91DE-175CB1D5A123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1785" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
   <si>
     <t>Jour</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Préparation du Sprint 2</t>
   </si>
   <si>
-    <t>Remplire l'analyse préliminaire</t>
-  </si>
-  <si>
     <t>Finaliser les stories du Sprint 2</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Choix et adaptation du template</t>
   </si>
   <si>
-    <t>Créer la connexion entre à la base de données et afiicher les biscuits</t>
-  </si>
-  <si>
     <t>Créer la page des détails</t>
   </si>
   <si>
@@ -147,12 +141,6 @@
     <t>Héberger une partie du site sur SwissCenter</t>
   </si>
   <si>
-    <t>Srpint Review</t>
-  </si>
-  <si>
-    <t>Ajouter des stratgies de test dans le rappot</t>
-  </si>
-  <si>
     <t>Améliorer l'aspect graphique du site</t>
   </si>
   <si>
@@ -198,9 +186,6 @@
     <t>Créer un menu de filtre sur la page boutique</t>
   </si>
   <si>
-    <t xml:space="preserve">Valider les commandes du panier et envoyer les données dans la base de donées </t>
-  </si>
-  <si>
     <t>Corriger des erreurs d'affichage des informations de l'utilisateur</t>
   </si>
   <si>
@@ -211,6 +196,33 @@
   </si>
   <si>
     <t>Mettre la nouvelle version sur SwissCenter</t>
+  </si>
+  <si>
+    <t>Tester le backend du site web</t>
+  </si>
+  <si>
+    <t>Héberger la version finale sur SwissCenter et tester son fonctionnement</t>
+  </si>
+  <si>
+    <t>Finaliser la documentation</t>
+  </si>
+  <si>
+    <t>Résolution de souci avec l'hébergement</t>
+  </si>
+  <si>
+    <t>Remplir l'analyse préliminaire</t>
+  </si>
+  <si>
+    <t>Créer la connexion entre à la base de données et afficher les biscuits</t>
+  </si>
+  <si>
+    <t>Ajouter des stratégies de test dans le rapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valider les commandes du panier et envoyer les données dans la base de données </t>
+  </si>
+  <si>
+    <t>Tester le frontend du site web</t>
   </si>
 </sst>
 </file>
@@ -613,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +890,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="F14" s="5"/>
     </row>
@@ -914,7 +926,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -929,10 +941,10 @@
         <v>2</v>
       </c>
       <c r="D17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -947,10 +959,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -965,10 +977,10 @@
         <v>0.5</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F19" s="5"/>
     </row>
@@ -983,10 +995,10 @@
         <v>2.5</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F20" s="5"/>
     </row>
@@ -1001,10 +1013,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F21" s="5"/>
     </row>
@@ -1019,10 +1031,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F22" s="5"/>
     </row>
@@ -1037,10 +1049,10 @@
         <v>2.25</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F23" s="5"/>
     </row>
@@ -1055,10 +1067,10 @@
         <v>1.5</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F24" s="5"/>
     </row>
@@ -1073,10 +1085,10 @@
         <v>1.5</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F25" s="5"/>
     </row>
@@ -1091,10 +1103,10 @@
         <v>2.25</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F26" s="5"/>
     </row>
@@ -1112,7 +1124,7 @@
         <v>18</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -1127,10 +1139,10 @@
         <v>0.5</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -1145,10 +1157,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29" s="5"/>
     </row>
@@ -1166,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="F30" s="5"/>
     </row>
@@ -1184,7 +1196,7 @@
         <v>18</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="F31" s="5"/>
     </row>
@@ -1199,10 +1211,10 @@
         <v>2.25</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F32" s="5"/>
     </row>
@@ -1217,10 +1229,10 @@
         <v>1.5</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F33" s="5"/>
     </row>
@@ -1235,10 +1247,10 @@
         <v>1.5</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F34" s="5"/>
     </row>
@@ -1253,10 +1265,10 @@
         <v>1.5</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F35" s="5"/>
     </row>
@@ -1271,10 +1283,10 @@
         <v>1</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F36" s="5"/>
     </row>
@@ -1292,7 +1304,7 @@
         <v>18</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F37" s="5"/>
     </row>
@@ -1307,10 +1319,10 @@
         <v>0.75</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F38" s="5"/>
     </row>
@@ -1328,7 +1340,7 @@
         <v>18</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F39" s="5"/>
     </row>
@@ -1346,7 +1358,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F40" s="5"/>
     </row>
@@ -1361,10 +1373,10 @@
         <v>2.25</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F41" s="5"/>
     </row>
@@ -1379,10 +1391,10 @@
         <v>0.75</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F42" s="5"/>
     </row>
@@ -1397,10 +1409,10 @@
         <v>0.75</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F43" s="5"/>
     </row>
@@ -1415,10 +1427,10 @@
         <v>0.5</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F44" s="5"/>
     </row>
@@ -1433,10 +1445,10 @@
         <v>1.5</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F45" s="5"/>
     </row>
@@ -1451,10 +1463,10 @@
         <v>1</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F46" s="5"/>
     </row>
@@ -1469,10 +1481,10 @@
         <v>1.5</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F47" s="5"/>
     </row>
@@ -1487,10 +1499,10 @@
         <v>1.5</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F48" s="5"/>
     </row>
@@ -1508,7 +1520,7 @@
         <v>18</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F49" s="5"/>
     </row>
@@ -1526,7 +1538,7 @@
         <v>18</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F50" s="5"/>
     </row>
@@ -1541,10 +1553,10 @@
         <v>1.5</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F51" s="5"/>
     </row>
@@ -1559,10 +1571,10 @@
         <v>1.5</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F52" s="5"/>
     </row>
@@ -1577,10 +1589,10 @@
         <v>1.5</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F53" s="5"/>
     </row>
@@ -1598,7 +1610,7 @@
         <v>18</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F54" s="5"/>
     </row>
@@ -1613,12 +1625,156 @@
         <v>1</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>45076</v>
+      </c>
+      <c r="B56" s="7">
+        <v>5</v>
+      </c>
+      <c r="C56" s="8">
+        <v>3</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>45076</v>
+      </c>
+      <c r="B57" s="7">
+        <v>5</v>
+      </c>
+      <c r="C57" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>45078</v>
+      </c>
+      <c r="B58" s="7">
+        <v>5</v>
+      </c>
+      <c r="C58" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>45078</v>
+      </c>
+      <c r="B59" s="7">
+        <v>5</v>
+      </c>
+      <c r="C59" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>45079</v>
+      </c>
+      <c r="B60" s="7">
+        <v>5</v>
+      </c>
+      <c r="C60" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>45079</v>
+      </c>
+      <c r="B61" s="7">
+        <v>5</v>
+      </c>
+      <c r="C61" s="8">
+        <v>1</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>45079</v>
+      </c>
+      <c r="B62" s="7">
+        <v>5</v>
+      </c>
+      <c r="C62" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>45079</v>
+      </c>
+      <c r="B63" s="7">
+        <v>5</v>
+      </c>
+      <c r="C63" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F63" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>